<commit_message>
edited the function to have a better sampled output
</commit_message>
<xml_diff>
--- a/validation/selectedPapers.xlsx
+++ b/validation/selectedPapers.xlsx
@@ -472,15 +472,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Spot pricing in the Cloud ecosystem: A comparative investigation</t>
+          <t>A systematic literature review and taxonomy of modern code review</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -488,145 +488,145 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="F2" t="n">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G2" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A systematic literature review on software measurement programs</t>
+          <t>A systematic literature review of how mutation testing supports quality assurance processes</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Information and Software Technology</t>
+          <t>Software Testing Verification and Reliability</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="F3" t="n">
-        <v>1997</v>
+        <v>1984</v>
       </c>
       <c r="G3" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>120</v>
+        <v>17</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Requirements for product derivation support: Results from a systematic literature review and an expert survey</t>
+          <t>A Systematic Literature Review of iStar extensions</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Information and Software Technology</t>
+          <t>Journal of Systems and Software</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F4" t="n">
-        <v>1996</v>
+        <v>1990</v>
       </c>
       <c r="G4" t="n">
-        <v>2007</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A systematic literature review on SOA migration</t>
+          <t>A systematic literature review of software visualization evaluation</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Journal of Software: Evolution and Process</t>
+          <t>Journal of Systems and Software</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>75</v>
+        <v>181</v>
       </c>
       <c r="F5" t="n">
-        <v>2000</v>
+        <v>2002</v>
       </c>
       <c r="G5" t="n">
-        <v>2013</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Systematic literature review of domain-oriented specification techniques</t>
+          <t>A systematic literature review of test breakage prevention and repair techniques</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Journal of Systems and Software</t>
+          <t>Information and Software Technology</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F6" t="n">
-        <v>1989</v>
+        <v>2003</v>
       </c>
       <c r="G6" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>164</v>
+        <v>25</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Training students in evidence-based software engineering and systematic reviews: a systematic review and empirical study</t>
+          <t>A systematic literature review on crowdsourcing in software engineering</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Empirical Software Engineering</t>
+          <t>Journal of Systems and Software</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="F7" t="n">
-        <v>2005</v>
+        <v>2009</v>
       </c>
       <c r="G7" t="n">
         <v>2018</v>
@@ -634,42 +634,42 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>167</v>
+        <v>30</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Variability in software systems-A systematic literature review</t>
+          <t>A systematic literature review on SOA migration</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>IEEE Transactions on Software Engineering</t>
+          <t>Journal of Software: Evolution and Process</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>196</v>
+        <v>75</v>
       </c>
       <c r="F8" t="n">
         <v>2000</v>
       </c>
       <c r="G8" t="n">
-        <v>2011</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>An extensive systematic review on the Model-Driven Development of secure systems</t>
+          <t>A systematic literature review on software measurement programs</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -677,10 +677,10 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="F9" t="n">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="G9" t="n">
         <v>2014</v>
@@ -688,96 +688,96 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Meta-analysis for families of experiments in software engineering: a systematic review and reproducibility and validity assessment</t>
+          <t>A systematic literature review on Technical Debt prioritization: Strategies, processes, factors, and tools</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Empirical Software Engineering</t>
+          <t>Journal of Systems and Software</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="F10" t="n">
-        <v>2001</v>
+        <v>2011</v>
       </c>
       <c r="G10" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Approaches to manage the user experience process in Agile software development: A systematic literature review</t>
+          <t>A Taxonomy and Qualitative Comparison of Program Analysis Techniques for Security Assessment of Android Software</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Information and Software Technology</t>
+          <t>IEEE Transactions on Software Engineering</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>49</v>
+        <v>336</v>
       </c>
       <c r="F11" t="n">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="G11" t="n">
-        <v>2019</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A systematic literature review of how mutation testing supports quality assurance processes</t>
+          <t>An extensive systematic review on the Model-Driven Development of secure systems</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Software Testing Verification and Reliability</t>
+          <t>Information and Software Technology</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>191</v>
+        <v>124</v>
       </c>
       <c r="F12" t="n">
-        <v>1984</v>
+        <v>2002</v>
       </c>
       <c r="G12" t="n">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>159</v>
+        <v>61</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Time pressure in software engineering: A systematic review</t>
+          <t>Approaches to manage the user experience process in Agile software development: A systematic literature review</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -785,53 +785,53 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>1984</v>
+        <v>2007</v>
       </c>
       <c r="G13" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>136</v>
+        <v>69</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Software project scheduling problem in the context of search-based software engineering: A systematic review</t>
+          <t>Business process maturity models: A systematic literature review</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Journal of Systems and Software</t>
+          <t>Information and Software Technology</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="F14" t="n">
-        <v>1998</v>
+        <v>2001</v>
       </c>
       <c r="G14" t="n">
-        <v>2018</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A Taxonomy and Qualitative Comparison of Program Analysis Techniques for Security Assessment of Android Software</t>
+          <t>Comparing Methods for Large-Scale Agile Software Development: A Systematic Literature Review</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -839,26 +839,26 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>336</v>
+        <v>191</v>
       </c>
       <c r="F15" t="n">
-        <v>2009</v>
+        <v>2003</v>
       </c>
       <c r="G15" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Business process maturity models: A systematic literature review</t>
+          <t>Empirical studies of agile software development: A systematic review</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -866,67 +866,67 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="F16" t="n">
         <v>2001</v>
       </c>
       <c r="G16" t="n">
-        <v>2014</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Empirical studies of agile software development: A systematic review</t>
+          <t>Meta-analysis for families of experiments in software engineering: a systematic review and reproducibility and validity assessment</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Information and Software Technology</t>
+          <t>Empirical Software Engineering</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="F17" t="n">
         <v>2001</v>
       </c>
       <c r="G17" t="n">
-        <v>2005</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>A systematic literature review on crowdsourcing in software engineering</t>
+          <t>Multicloud service composition: A survey of current approaches and issues</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Journal of Systems and Software</t>
+          <t>Journal of Software: Evolution and Process</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="F18" t="n">
-        <v>2009</v>
+        <v>2013</v>
       </c>
       <c r="G18" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="19">
@@ -958,96 +958,96 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Comparing Methods for Large-Scale Agile Software Development: A Systematic Literature Review</t>
+          <t>Requirements for product derivation support: Results from a systematic literature review and an expert survey</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2022</v>
+        <v>2010</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>IEEE Transactions on Software Engineering</t>
+          <t>Information and Software Technology</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="F20" t="n">
-        <v>2003</v>
+        <v>1996</v>
       </c>
       <c r="G20" t="n">
-        <v>2019</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Multicloud service composition: A survey of current approaches and issues</t>
+          <t>Software project scheduling problem in the context of search-based software engineering: A systematic review</t>
         </is>
       </c>
       <c r="C21" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Journal of Systems and Software</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>37</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1998</v>
+      </c>
+      <c r="G21" t="n">
         <v>2018</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Journal of Software: Evolution and Process</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>21</v>
-      </c>
-      <c r="F21" t="n">
-        <v>2013</v>
-      </c>
-      <c r="G21" t="n">
-        <v>2017</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A systematic literature review of test breakage prevention and repair techniques</t>
+          <t>Spot pricing in the Cloud ecosystem: A comparative investigation</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Information and Software Technology</t>
+          <t>Journal of Systems and Software</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="F22" t="n">
-        <v>2003</v>
+        <v>2010</v>
       </c>
       <c r="G22" t="n">
-        <v>2018</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>A Systematic Literature Review of iStar extensions</t>
+          <t>Systematic literature review of domain-oriented specification techniques</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1055,94 +1055,94 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="F23" t="n">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="G23" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>A systematic literature review on Technical Debt prioritization: Strategies, processes, factors, and tools</t>
+          <t>Time pressure in software engineering: A systematic review</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Journal of Systems and Software</t>
+          <t>Information and Software Technology</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="F24" t="n">
-        <v>2011</v>
+        <v>1984</v>
       </c>
       <c r="G24" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>A systematic literature review of software visualization evaluation</t>
+          <t>Training students in evidence-based software engineering and systematic reviews: a systematic review and empirical study</t>
         </is>
       </c>
       <c r="C25" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Empirical Software Engineering</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>14</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2005</v>
+      </c>
+      <c r="G25" t="n">
         <v>2018</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Journal of Systems and Software</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>181</v>
-      </c>
-      <c r="F25" t="n">
-        <v>2002</v>
-      </c>
-      <c r="G25" t="n">
-        <v>2017</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>13</v>
+        <v>167</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A systematic literature review and taxonomy of modern code review</t>
+          <t>Variability in software systems-A systematic literature review</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2021</v>
+        <v>2014</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Journal of Systems and Software</t>
+          <t>IEEE Transactions on Software Engineering</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="F26" t="n">
-        <v>2009</v>
+        <v>2000</v>
       </c>
       <c r="G26" t="n">
-        <v>2019</v>
+        <v>2011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited script to make the selected sample size easier to read and added new columns
</commit_message>
<xml_diff>
--- a/validation/selectedPapers.xlsx
+++ b/validation/selectedPapers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,16 @@
           <t>The latest year of the reviewed papers</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>research_question</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>search_string</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -496,6 +506,8 @@
       <c r="G2" t="n">
         <v>2019</v>
       </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -523,6 +535,8 @@
       <c r="G3" t="n">
         <v>2015</v>
       </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -550,6 +564,8 @@
       <c r="G4" t="n">
         <v>2016</v>
       </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -577,6 +593,8 @@
       <c r="G5" t="n">
         <v>2017</v>
       </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -604,6 +622,8 @@
       <c r="G6" t="n">
         <v>2018</v>
       </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -631,6 +651,8 @@
       <c r="G7" t="n">
         <v>2018</v>
       </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -658,6 +680,8 @@
       <c r="G8" t="n">
         <v>2013</v>
       </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -685,6 +709,8 @@
       <c r="G9" t="n">
         <v>2014</v>
       </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -712,6 +738,8 @@
       <c r="G10" t="n">
         <v>2019</v>
       </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -739,6 +767,8 @@
       <c r="G11" t="n">
         <v>2015</v>
       </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -766,6 +796,8 @@
       <c r="G12" t="n">
         <v>2014</v>
       </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -793,6 +825,8 @@
       <c r="G13" t="n">
         <v>2019</v>
       </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -820,6 +854,8 @@
       <c r="G14" t="n">
         <v>2014</v>
       </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -847,6 +883,8 @@
       <c r="G15" t="n">
         <v>2019</v>
       </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -874,6 +912,8 @@
       <c r="G16" t="n">
         <v>2005</v>
       </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -901,6 +941,8 @@
       <c r="G17" t="n">
         <v>2016</v>
       </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -928,6 +970,8 @@
       <c r="G18" t="n">
         <v>2017</v>
       </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -955,6 +999,8 @@
       <c r="G19" t="n">
         <v>2011</v>
       </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -982,6 +1028,8 @@
       <c r="G20" t="n">
         <v>2007</v>
       </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1009,6 +1057,8 @@
       <c r="G21" t="n">
         <v>2018</v>
       </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1036,6 +1086,8 @@
       <c r="G22" t="n">
         <v>2015</v>
       </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1063,6 +1115,8 @@
       <c r="G23" t="n">
         <v>2019</v>
       </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1090,6 +1144,8 @@
       <c r="G24" t="n">
         <v>2017</v>
       </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1117,6 +1173,8 @@
       <c r="G25" t="n">
         <v>2018</v>
       </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1144,6 +1202,8 @@
       <c r="G26" t="n">
         <v>2011</v>
       </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added more dataentries and a script that extract only valid data entries from the dataset
</commit_message>
<xml_diff>
--- a/validation/selectedPapers.xlsx
+++ b/validation/selectedPapers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodol\OneDrive\Documents\SE-ALL\SearchStringAI\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0947FDC8-956E-4B6F-B08D-4C66A7733830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D54B64-F7F2-4DE4-85CC-A62A48761F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-86" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="264">
   <si>
     <t>ID</t>
   </si>
@@ -590,9 +590,6 @@
   </si>
   <si>
     <t>What factors, as identified in the informal literature review, have a positive impact on implementing SPI? What factors, as identified in the formal literature review, have a positive impact on implementing SPI? What factors, as identified in the empirical study, have a positive impact on implementing SPI? How are these factors related to the methodology used?</t>
-  </si>
-  <si>
-    <t>Note</t>
   </si>
   <si>
     <t>What are the challenges of managing software maintenance in globally distributed settings? How do software organizations mitigate these challenges?</t>
@@ -2240,6 +2237,62 @@
   <si>
     <t xml:space="preserve">RQ1: What are the inputs used by SIAs? RQ2: What are the processes followed by SIAs? RQ3: What are the outputs of SIAs? 
 RQ4: What is the usability of SIAs? </t>
+  </si>
+  <si>
+    <t>(service identification OR service mining OR service packaging) AND (migration OR modernization OR transformation OR re-engineering) AND (legacy OR existing systems OR Object-Oriented)</t>
+  </si>
+  <si>
+    <t>(agile AND practice AND select) OR
+(agile AND method AND tailoring) OR
+(scrum AND practice AND adoption) OR
+(scrum AND tailoring) OR
+(scrum AND practice AND select) OR
+(xp AND practice AND adoption) OR
+(xp AND tailoring) OR
+(xp AND practice AND select) OR
+(kanban AND practice AND adoption) OR
+(kanban AND tailoring) OR
+(kanban AND practice AND select) OR
+(lean AND practice AND adoption) OR
+(lean AND tailoring) OR
+(lean AND practice AND select) OR
+(fdd AND practice AND adoption) OR
+(fdd AND tailoring) OR
+(fdd AND practice AND select) OR
+(“feature driven development” AND practice AND adoption) OR
+(“feature driven development” AND tailoring) OR
+(“feature driven development” AND practice AND select)</t>
+  </si>
+  <si>
+    <t>RQ1	What are the methodological aspects of agile method tailoring research?
+RQ2	How practical has agile methods tailoring research been?
+RQ3	Which are the method tailoring criteria used for agile methods tailoring?</t>
+  </si>
+  <si>
+    <t>RQ1: What are the agile practices for the CSFs, as identified in the literature, to be adapted by the GSD vendors in the development of green and sustainable software?
+RQ2: What are the agile practices for the CSFs, as identified in the real-world practice, to be adapted by the GSD vendors in the development of green and sustainable software?</t>
+  </si>
+  <si>
+    <t>(“Green software” OR “Greener software” OR “Sustainable software” OR “Green software engineering”) AND (“Agile” OR “Agile methods” OR “green agile”) AND (“Practices” OR “Solutions”)</t>
+  </si>
+  <si>
+    <t>(Agile OR Agility OR Scrum OR "eXtreme Programming") AND (CMMI OR "Capability Maturity Model") AND (Web OR "Web Engineering")</t>
+  </si>
+  <si>
+    <t>RQ1: What is the relation between CMMI-DEV maturity levels and Agile methodologies in Web environments?
+RQ2: What evaluation criterion concludes that an Agile technique is compliant with certain goals of a CMMI-DEV process area in Web environments?
+RQ3: What experiments or case studies could validate an Agile approach to maturity models in Web environments?
+RQ4: What is the highest documented maturity level that can be reached using Agile approaches in Web environments?
+RQ5: How could Web specific characteristics be addressed through Agile methods so as to reach CMMI-DEV goals?</t>
+  </si>
+  <si>
+    <t>What types of data collection methods have been used in the studies? What curriculum models (bodies of knowledge) have been used to design the studies? Which SE skills (subjects) are the most important and which SE subjects are the least important for a typical software engineer in practice? What is the evidence for knowledge gaps (deficiencies) in different SE subjects? And what are the topics with the highest knowledge deficiencies? What is the evidence on the importance of soft skills? And to what extent are soft skills important, in addition to technical (“hard”) skills?What are the characteristics of the data sample? For example, what is the number of data points (e.g., participants, job advertisements) in the survey conducted by a given study? Which region (countries) are covered by the surveys? What educational recommendations are provided in each study? How do the findings of our meta-analysis (importance of SE skills, and knowledge gaps) compare to the findings of previous review papers (Radermacher, 2012; Radermacher and Walia, 2013; Aničić et al., 2017) (which had similar objectives), as discussed in Section 2?</t>
+  </si>
+  <si>
+    <t>(educational needs OR knowledge needs OR desired skills OR essential competencies OR knowledge requirements OR skill requirements) AND (software engineers OR software developers)</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -2391,7 +2444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2415,7 +2468,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2429,16 +2482,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2746,8 +2803,8 @@
   </sheetPr>
   <dimension ref="A1:L171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -2785,11 +2842,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>231</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>7</v>
@@ -2798,7 +2855,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>190</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1">
@@ -2882,10 +2939,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K4" t="s">
         <v>191</v>
-      </c>
-      <c r="K4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75" customHeight="1">
@@ -2914,7 +2971,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18.75" customHeight="1">
@@ -2966,7 +3023,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18.75" customHeight="1">
@@ -2995,10 +3052,10 @@
         <v>5</v>
       </c>
       <c r="J8" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="L8" t="s">
         <v>195</v>
-      </c>
-      <c r="L8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="18.75" customHeight="1">
@@ -3030,10 +3087,10 @@
         <v>3</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18.75" customHeight="1">
@@ -3062,7 +3119,7 @@
         <v>6</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18.75" customHeight="1">
@@ -3094,10 +3151,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" customHeight="1">
@@ -3129,10 +3186,10 @@
         <v>1</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K12" t="s">
         <v>202</v>
-      </c>
-      <c r="K12" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1">
@@ -3164,10 +3221,10 @@
         <v>1</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" customHeight="1">
@@ -3199,10 +3256,10 @@
         <v>1</v>
       </c>
       <c r="J14" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1">
@@ -3234,10 +3291,10 @@
         <v>1</v>
       </c>
       <c r="J15" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18.75" customHeight="1">
@@ -3269,13 +3326,13 @@
         <v>1</v>
       </c>
       <c r="J16" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="L16" t="s">
         <v>211</v>
-      </c>
-      <c r="L16" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="18.75" customHeight="1">
@@ -3304,7 +3361,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="18.75" customHeight="1">
@@ -3333,7 +3390,7 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" customHeight="1">
@@ -3477,7 +3534,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="18.75" customHeight="1">
@@ -3506,10 +3563,10 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="18.75" customHeight="1">
@@ -3570,7 +3627,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="18.75" customHeight="1">
@@ -3602,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="18.75" customHeight="1">
@@ -3634,7 +3691,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="18.75" customHeight="1">
@@ -3666,7 +3723,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="18.75" customHeight="1">
@@ -3698,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="18.75" customHeight="1">
@@ -3730,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="18.75" customHeight="1">
@@ -3762,7 +3819,7 @@
         <v>1</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="18.75" customHeight="1">
@@ -3794,10 +3851,10 @@
         <v>1</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="18.75" customHeight="1">
@@ -3829,10 +3886,10 @@
         <v>1</v>
       </c>
       <c r="J35" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="K35" s="19" t="s">
         <v>227</v>
-      </c>
-      <c r="K35" s="20" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="18.75" customHeight="1">
@@ -3864,10 +3921,10 @@
         <v>1</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="18.75" customHeight="1">
@@ -3899,10 +3956,10 @@
         <v>1</v>
       </c>
       <c r="J37" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="K37" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="18.75" customHeight="1">
@@ -3931,13 +3988,13 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J38" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="K38" t="s">
         <v>235</v>
-      </c>
-      <c r="K38" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="18.75" customHeight="1">
@@ -3969,10 +4026,10 @@
         <v>4</v>
       </c>
       <c r="J39" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L39" t="s">
         <v>237</v>
-      </c>
-      <c r="L39" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="18.75" customHeight="1">
@@ -4004,13 +4061,13 @@
         <v>1</v>
       </c>
       <c r="J40" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="K40" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="K40" s="6" t="s">
+      <c r="L40" t="s">
         <v>240</v>
-      </c>
-      <c r="L40" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="18.75" customHeight="1">
@@ -4042,10 +4099,10 @@
         <v>1</v>
       </c>
       <c r="J41" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="K41" t="s">
         <v>242</v>
-      </c>
-      <c r="K41" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="18.75" customHeight="1">
@@ -4071,19 +4128,19 @@
         <v>2006</v>
       </c>
       <c r="H42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="18.75" customHeight="1">
@@ -4115,10 +4172,10 @@
         <v>1</v>
       </c>
       <c r="J43" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="K43" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="18.75" customHeight="1">
@@ -4150,10 +4207,10 @@
         <v>1</v>
       </c>
       <c r="J44" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="K44" t="s">
         <v>247</v>
-      </c>
-      <c r="K44" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="18.75" customHeight="1">
@@ -4185,10 +4242,10 @@
         <v>1</v>
       </c>
       <c r="J45" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="K45" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="18.75" customHeight="1">
@@ -4217,13 +4274,13 @@
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J46" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="K46" t="s">
         <v>251</v>
-      </c>
-      <c r="K46" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="18.75" customHeight="1">
@@ -4252,10 +4309,10 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="18.75" customHeight="1">
@@ -4280,11 +4337,20 @@
       <c r="G48" s="3">
         <v>2019</v>
       </c>
+      <c r="H48" s="20">
+        <v>4</v>
+      </c>
+      <c r="I48" s="21">
+        <v>1</v>
+      </c>
       <c r="J48" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="K48" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="18.75" customHeight="1">
+    <row r="49" spans="1:11" ht="18.75" customHeight="1">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4306,8 +4372,20 @@
       <c r="G49" s="3">
         <v>2014</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="18.75" customHeight="1">
+      <c r="H49" s="20">
+        <v>3</v>
+      </c>
+      <c r="I49" s="21">
+        <v>1</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="18.75" customHeight="1">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4329,8 +4407,20 @@
       <c r="G50" s="3">
         <v>2015</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="18.75" customHeight="1">
+      <c r="H50" s="20">
+        <v>2</v>
+      </c>
+      <c r="I50" s="21">
+        <v>1</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="K50" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="18.75" customHeight="1">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4352,8 +4442,20 @@
       <c r="G51" s="3">
         <v>2014</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="18.75" customHeight="1">
+      <c r="H51" s="20">
+        <v>5</v>
+      </c>
+      <c r="I51" s="21">
+        <v>1</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="K51" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="18.75" customHeight="1">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4375,8 +4477,20 @@
       <c r="G52" s="3">
         <v>2018</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="18.75" customHeight="1">
+      <c r="H52" s="20">
+        <v>8</v>
+      </c>
+      <c r="I52" s="21">
+        <v>1</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K52" s="22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="18.75" customHeight="1">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -4399,7 +4513,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="18.75" customHeight="1">
+    <row r="54" spans="1:11" ht="18.75" customHeight="1">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4422,7 +4536,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="18.75" customHeight="1">
+    <row r="55" spans="1:11" ht="18.75" customHeight="1">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4445,7 +4559,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18.75" customHeight="1">
+    <row r="56" spans="1:11" ht="18.75" customHeight="1">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4468,7 +4582,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18.75" customHeight="1">
+    <row r="57" spans="1:11" ht="18.75" customHeight="1">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4491,7 +4605,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="18.75" customHeight="1">
+    <row r="58" spans="1:11" ht="18.75" customHeight="1">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4514,7 +4628,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="18.75" customHeight="1">
+    <row r="59" spans="1:11" ht="18.75" customHeight="1">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4537,7 +4651,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="18.75" customHeight="1">
+    <row r="60" spans="1:11" ht="18.75" customHeight="1">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4560,7 +4674,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="18.75" customHeight="1">
+    <row r="61" spans="1:11" ht="18.75" customHeight="1">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4583,7 +4697,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="18.75" customHeight="1">
+    <row r="62" spans="1:11" ht="18.75" customHeight="1">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4606,7 +4720,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="18.75" customHeight="1">
+    <row r="63" spans="1:11" ht="18.75" customHeight="1">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4629,7 +4743,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="18.75" customHeight="1">
+    <row r="64" spans="1:11" ht="18.75" customHeight="1">
       <c r="A64" s="3">
         <v>63</v>
       </c>

</xml_diff>